<commit_message>
MAJ Fiche de séquence Informatique
</commit_message>
<xml_diff>
--- a/Progression/Progression_Informatique_2014_2015.xlsx
+++ b/Progression/Progression_Informatique_2014_2015.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="11670" windowHeight="7860" activeTab="3"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="269">
   <si>
     <t>01/09/2014
 au
@@ -1117,9 +1117,6 @@
     <t>Introduction à l'algorithmique et à la programmation.</t>
   </si>
   <si>
-    <t>Horaire élève</t>
-  </si>
-  <si>
     <t>Activité</t>
   </si>
   <si>
@@ -1141,121 +1138,333 @@
     <t>11 heures</t>
   </si>
   <si>
-    <t>Séance 1 et 2</t>
-  </si>
-  <si>
-    <t>Séance 5</t>
-  </si>
-  <si>
-    <t>Séance 3 et 4</t>
-  </si>
-  <si>
-    <t>Séance 6</t>
-  </si>
-  <si>
-    <t>Séance 7</t>
-  </si>
-  <si>
     <t>TD d'application</t>
+  </si>
+  <si>
+    <t>Objectifs</t>
+  </si>
+  <si>
+    <t>Contenu</t>
+  </si>
+  <si>
+    <t>Décourir l'environnement Pyhon
+Découvrir les différents types de variables</t>
+  </si>
+  <si>
+    <t>Evaluation formative</t>
+  </si>
+  <si>
+    <t>Evaluation sommative</t>
+  </si>
+  <si>
+    <t>Découverte de l'interpréteur
+Découverte de l'éditeur
+Découverte des boucles
+Jeu du plus et moins
+Heures, minutes, secondes</t>
+  </si>
+  <si>
+    <t>Découverte des listes
+Découverte d'un premier algorithme de recherche
+Tracer des courbes</t>
+  </si>
+  <si>
+    <t>Courbe de polaire d'un profil d'une aile d'avion
+Tracer d'une courbe paramétrique
+Projet Solar Pi</t>
+  </si>
+  <si>
+    <t>Activités &amp; Compétences</t>
+  </si>
+  <si>
+    <t>Synnthèse sur les notions de variables, et expressions</t>
+  </si>
+  <si>
+    <t>Exemple : Algorithme d'Euclide
+Variables
+Expressions</t>
+  </si>
+  <si>
+    <t>Synthèse sur les fonctions et structures algorithmiques.</t>
+  </si>
+  <si>
+    <t>Exemple : Courbes de Bézier
+Rudiments
+Instructions conditionnelles
+Instructions ittératives</t>
+  </si>
+  <si>
+    <t>QCM 1, 2 et 3</t>
+  </si>
+  <si>
+    <t>Valider les compétences acquises à la séance de TP précédente.</t>
+  </si>
+  <si>
+    <t>Devoir surveillé 1</t>
+  </si>
+  <si>
+    <t>Horaires élève</t>
+  </si>
+  <si>
+    <t>ORGANISATION ELEVES</t>
+  </si>
+  <si>
+    <t>ORGANISATION PEDAGOGIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANALYSER le codage des nombres.
+ANALYSER un algorithme est expliquer ce qu'il fait. </t>
+  </si>
+  <si>
+    <t>Séances 1 et 2 (4 h)</t>
+  </si>
+  <si>
+    <t>Séances 3 et 4 (4h)</t>
+  </si>
+  <si>
+    <t>Séance 6
+(1h)</t>
+  </si>
+  <si>
+    <t>Séance 5
+(1h)</t>
+  </si>
+  <si>
+    <t>Séance 7
+(1h)</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Découverte</t>
+      <t>TP Découverte</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> de la programmation</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> de la programmation
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Découverte</t>
+      <t>ANALYSER</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> de l'algorithmique</t>
+      <t xml:space="preserve"> un problème
+Alg - C3, Alg - C5</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Synthèse</t>
+      <t>TP Découverte</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> programmation</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve"> de l'algorithmique
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Synthèse</t>
+      <t>ANALYSER</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> algorithmique</t>
+      <t xml:space="preserve"> et </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MODELISER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> une situation
+Alg - C2, Alg - C3, Ing - C3, Ing - C4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COURS Synthèse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> programmation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANALYSER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Alg - C1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COURS Synthèse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> algorithmique
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANALYSER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> et </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MODELISER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> une situation
+Alg - C1, Alg - C3, Alg - C4, Alg - C5</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1294,8 +1503,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1344,8 +1585,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1900,11 +2165,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2166,6 +2565,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2262,8 +2706,150 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2354,6 +2940,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2388,6 +2975,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2563,14 +3151,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="48" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="48" customWidth="1"/>
@@ -2582,7 +3170,7 @@
     <col min="10" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="12" thickBot="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="14" t="s">
@@ -2602,11 +3190,11 @@
       </c>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="141" t="s">
         <v>157</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -2621,11 +3209,11 @@
       </c>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75">
+    <row r="3" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="119"/>
+      <c r="B3" s="142"/>
       <c r="C3" s="25" t="s">
         <v>47</v>
       </c>
@@ -2636,11 +3224,11 @@
       <c r="F3" s="28"/>
       <c r="G3" s="29"/>
     </row>
-    <row r="4" spans="1:8" ht="33.75">
+    <row r="4" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="119"/>
+      <c r="B4" s="142"/>
       <c r="C4" s="31" t="s">
         <v>184</v>
       </c>
@@ -2653,11 +3241,11 @@
       <c r="F4" s="33"/>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:8" ht="33.75">
+    <row r="5" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="119"/>
+      <c r="B5" s="142"/>
       <c r="C5" s="25" t="s">
         <v>50</v>
       </c>
@@ -2670,11 +3258,11 @@
       <c r="F5" s="33"/>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:8" ht="33.75">
+    <row r="6" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="119"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="25" t="s">
         <v>51</v>
       </c>
@@ -2692,11 +3280,11 @@
       </c>
       <c r="H6" s="39"/>
     </row>
-    <row r="7" spans="1:8" ht="56.25">
+    <row r="7" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="119"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="25" t="s">
         <v>52</v>
       </c>
@@ -2714,11 +3302,11 @@
       </c>
       <c r="H7" s="42"/>
     </row>
-    <row r="8" spans="1:8" ht="34.5" thickBot="1">
+    <row r="8" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="120"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="44" t="s">
         <v>52</v>
       </c>
@@ -2729,49 +3317,49 @@
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
     </row>
-    <row r="9" spans="1:8" ht="12" thickBot="1">
+    <row r="9" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="49"/>
       <c r="D9" s="88"/>
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
       <c r="G9" s="49"/>
     </row>
-    <row r="10" spans="1:8" ht="33.75">
+    <row r="10" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="120" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="99"/>
-    </row>
-    <row r="11" spans="1:8" ht="34.5" thickBot="1">
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="122"/>
+    </row>
+    <row r="11" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-    </row>
-    <row r="12" spans="1:8" ht="12" thickBot="1">
+      <c r="B11" s="123"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="125"/>
+    </row>
+    <row r="12" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="49"/>
       <c r="D12" s="88"/>
       <c r="E12" s="49"/>
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
     </row>
-    <row r="13" spans="1:8" ht="33.75">
+    <row r="13" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="126" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -2790,11 +3378,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="33.75">
+    <row r="14" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="104"/>
+      <c r="B14" s="127"/>
       <c r="C14" s="36" t="s">
         <v>159</v>
       </c>
@@ -2805,11 +3393,11 @@
       <c r="F14" s="56"/>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:8" ht="56.25">
+    <row r="15" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="104"/>
+      <c r="B15" s="127"/>
       <c r="C15" s="36" t="s">
         <v>160</v>
       </c>
@@ -2826,11 +3414,11 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="33.75">
+    <row r="16" spans="1:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="104"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="40" t="s">
         <v>161</v>
       </c>
@@ -2841,11 +3429,11 @@
       <c r="F16" s="56"/>
       <c r="G16" s="29"/>
     </row>
-    <row r="17" spans="1:7" ht="45">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="104"/>
+      <c r="B17" s="127"/>
       <c r="C17" s="40" t="s">
         <v>161</v>
       </c>
@@ -2862,11 +3450,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="33.75">
+    <row r="18" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="104"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="40" t="s">
         <v>162</v>
       </c>
@@ -2881,11 +3469,11 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="34.5" thickBot="1">
+    <row r="19" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="105"/>
+      <c r="B19" s="128"/>
       <c r="C19" s="58" t="s">
         <v>162</v>
       </c>
@@ -2898,49 +3486,49 @@
       <c r="F19" s="61"/>
       <c r="G19" s="47"/>
     </row>
-    <row r="20" spans="1:7" ht="12" thickBot="1">
+    <row r="20" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C20" s="49"/>
       <c r="D20" s="88"/>
       <c r="E20" s="49"/>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
     </row>
-    <row r="21" spans="1:7" ht="33.75">
+    <row r="21" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="98"/>
-      <c r="F21" s="98"/>
-      <c r="G21" s="99"/>
-    </row>
-    <row r="22" spans="1:7" ht="34.5" thickBot="1">
+      <c r="C21" s="121"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="122"/>
+    </row>
+    <row r="22" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102"/>
-    </row>
-    <row r="23" spans="1:7" ht="12" thickBot="1">
+      <c r="B22" s="123"/>
+      <c r="C22" s="124"/>
+      <c r="D22" s="124"/>
+      <c r="E22" s="124"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="125"/>
+    </row>
+    <row r="23" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="49"/>
       <c r="D23" s="88"/>
       <c r="E23" s="49"/>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
     </row>
-    <row r="24" spans="1:7" ht="33.75">
+    <row r="24" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="126" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -2955,11 +3543,11 @@
       <c r="F24" s="52"/>
       <c r="G24" s="62"/>
     </row>
-    <row r="25" spans="1:7" ht="33.75">
+    <row r="25" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="104"/>
+      <c r="B25" s="127"/>
       <c r="C25" s="36" t="s">
         <v>168</v>
       </c>
@@ -2970,11 +3558,11 @@
       <c r="F25" s="56"/>
       <c r="G25" s="29"/>
     </row>
-    <row r="26" spans="1:7" ht="34.5" thickBot="1">
+    <row r="26" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="105"/>
+      <c r="B26" s="128"/>
       <c r="C26" s="64" t="s">
         <v>177</v>
       </c>
@@ -2987,11 +3575,11 @@
       <c r="F26" s="61"/>
       <c r="G26" s="47"/>
     </row>
-    <row r="27" spans="1:7" ht="45">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="129" t="s">
         <v>158</v>
       </c>
       <c r="C27" s="65" t="s">
@@ -3006,11 +3594,11 @@
       <c r="F27" s="66"/>
       <c r="G27" s="67"/>
     </row>
-    <row r="28" spans="1:7" ht="33.75">
+    <row r="28" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="106"/>
+      <c r="B28" s="129"/>
       <c r="C28" s="68" t="s">
         <v>170</v>
       </c>
@@ -3023,11 +3611,11 @@
       <c r="F28" s="56"/>
       <c r="G28" s="29"/>
     </row>
-    <row r="29" spans="1:7" ht="45">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="106"/>
+      <c r="B29" s="129"/>
       <c r="C29" s="68" t="s">
         <v>171</v>
       </c>
@@ -3042,11 +3630,11 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="34.5" thickBot="1">
+    <row r="30" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="107"/>
+      <c r="B30" s="130"/>
       <c r="C30" s="71" t="s">
         <v>171</v>
       </c>
@@ -3059,62 +3647,62 @@
       <c r="F30" s="61"/>
       <c r="G30" s="47"/>
     </row>
-    <row r="31" spans="1:7" ht="12" thickBot="1">
+    <row r="31" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="49"/>
       <c r="D31" s="88"/>
       <c r="E31" s="49"/>
       <c r="F31" s="49"/>
       <c r="G31" s="49"/>
     </row>
-    <row r="32" spans="1:7" ht="33.75">
+    <row r="32" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A32" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="97" t="s">
+      <c r="B32" s="120" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="99"/>
-    </row>
-    <row r="33" spans="1:7" ht="34.5" thickBot="1">
+      <c r="C32" s="121"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="121"/>
+      <c r="G32" s="122"/>
+    </row>
+    <row r="33" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="100"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="102"/>
-    </row>
-    <row r="34" spans="1:7" ht="12" thickBot="1">
+      <c r="B33" s="123"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="125"/>
+    </row>
+    <row r="34" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="49"/>
       <c r="D34" s="88"/>
       <c r="E34" s="49"/>
       <c r="F34" s="49"/>
       <c r="G34" s="49"/>
     </row>
-    <row r="35" spans="1:7" ht="36" customHeight="1" thickBot="1">
+    <row r="35" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="115" t="s">
+      <c r="B35" s="138" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="116"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="117"/>
-    </row>
-    <row r="36" spans="1:7" ht="61.5" customHeight="1">
+      <c r="C35" s="139"/>
+      <c r="D35" s="139"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="140"/>
+    </row>
+    <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="112" t="s">
+      <c r="B36" s="135" t="s">
         <v>158</v>
       </c>
       <c r="C36" s="74" t="s">
@@ -3129,11 +3717,11 @@
       <c r="F36" s="75"/>
       <c r="G36" s="66"/>
     </row>
-    <row r="37" spans="1:7" ht="33.75">
+    <row r="37" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="113"/>
+      <c r="B37" s="136"/>
       <c r="C37" s="76" t="s">
         <v>172</v>
       </c>
@@ -3146,11 +3734,11 @@
       <c r="F37" s="77"/>
       <c r="G37" s="56"/>
     </row>
-    <row r="38" spans="1:7" ht="33.75">
+    <row r="38" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="113"/>
+      <c r="B38" s="136"/>
       <c r="C38" s="78" t="s">
         <v>174</v>
       </c>
@@ -3163,11 +3751,11 @@
       <c r="F38" s="77"/>
       <c r="G38" s="56"/>
     </row>
-    <row r="39" spans="1:7" ht="33.75">
+    <row r="39" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="113"/>
+      <c r="B39" s="136"/>
       <c r="C39" s="78" t="s">
         <v>173</v>
       </c>
@@ -3180,11 +3768,11 @@
       <c r="F39" s="77"/>
       <c r="G39" s="56"/>
     </row>
-    <row r="40" spans="1:7" ht="33.75">
+    <row r="40" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="113"/>
+      <c r="B40" s="136"/>
       <c r="C40" s="78" t="s">
         <v>173</v>
       </c>
@@ -3199,11 +3787,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="34.5" thickBot="1">
+    <row r="41" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="114"/>
+      <c r="B41" s="137"/>
       <c r="C41" s="79" t="s">
         <v>175</v>
       </c>
@@ -3216,49 +3804,49 @@
       <c r="F41" s="80"/>
       <c r="G41" s="61"/>
     </row>
-    <row r="42" spans="1:7" ht="12" thickBot="1">
+    <row r="42" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C42" s="49"/>
       <c r="D42" s="88"/>
       <c r="E42" s="49"/>
       <c r="F42" s="49"/>
       <c r="G42" s="49"/>
     </row>
-    <row r="43" spans="1:7" ht="33.75">
+    <row r="43" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A43" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="97" t="s">
+      <c r="B43" s="120" t="s">
         <v>166</v>
       </c>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="99"/>
-    </row>
-    <row r="44" spans="1:7" ht="34.5" thickBot="1">
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="122"/>
+    </row>
+    <row r="44" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="100"/>
-      <c r="C44" s="101"/>
-      <c r="D44" s="101"/>
-      <c r="E44" s="101"/>
-      <c r="F44" s="101"/>
-      <c r="G44" s="102"/>
-    </row>
-    <row r="45" spans="1:7" ht="12" thickBot="1">
+      <c r="B44" s="123"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="124"/>
+      <c r="E44" s="124"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="125"/>
+    </row>
+    <row r="45" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="49"/>
       <c r="D45" s="88"/>
       <c r="E45" s="49"/>
       <c r="F45" s="49"/>
       <c r="G45" s="49"/>
     </row>
-    <row r="46" spans="1:7" ht="36" customHeight="1">
+    <row r="46" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="134" t="s">
         <v>158</v>
       </c>
       <c r="C46" s="83" t="s">
@@ -3271,11 +3859,11 @@
       <c r="F46" s="52"/>
       <c r="G46" s="62"/>
     </row>
-    <row r="47" spans="1:7" ht="33.75">
+    <row r="47" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="106"/>
+      <c r="B47" s="129"/>
       <c r="C47" s="69" t="s">
         <v>179</v>
       </c>
@@ -3286,11 +3874,11 @@
       <c r="F47" s="56"/>
       <c r="G47" s="29"/>
     </row>
-    <row r="48" spans="1:7" ht="34.5" thickBot="1">
+    <row r="48" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="107"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="69" t="s">
         <v>179</v>
       </c>
@@ -3301,11 +3889,11 @@
       <c r="F48" s="56"/>
       <c r="G48" s="29"/>
     </row>
-    <row r="49" spans="1:7" ht="33.75">
+    <row r="49" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="108" t="s">
+      <c r="B49" s="131" t="s">
         <v>167</v>
       </c>
       <c r="C49" s="85" t="s">
@@ -3320,11 +3908,11 @@
       <c r="F49" s="56"/>
       <c r="G49" s="29"/>
     </row>
-    <row r="50" spans="1:7" ht="33.75">
+    <row r="50" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A50" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="109"/>
+      <c r="B50" s="132"/>
       <c r="C50" s="85" t="s">
         <v>176</v>
       </c>
@@ -3339,11 +3927,11 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="33.75">
+    <row r="51" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="109"/>
+      <c r="B51" s="132"/>
       <c r="C51" s="85" t="s">
         <v>176</v>
       </c>
@@ -3356,11 +3944,11 @@
       <c r="F51" s="56"/>
       <c r="G51" s="29"/>
     </row>
-    <row r="52" spans="1:7" ht="34.5" thickBot="1">
+    <row r="52" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="110"/>
+      <c r="B52" s="133"/>
       <c r="C52" s="86" t="s">
         <v>179</v>
       </c>
@@ -3373,29 +3961,29 @@
       <c r="F52" s="61"/>
       <c r="G52" s="47"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C53" s="49"/>
       <c r="D53" s="88"/>
       <c r="E53" s="49"/>
       <c r="F53" s="49"/>
       <c r="G53" s="49"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C56" s="23" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C57" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C58" s="34" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C59" s="35" t="s">
         <v>139</v>
       </c>
@@ -3421,41 +4009,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -3467,30 +4055,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D62"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A55" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:D54"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="40.42578125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="12" thickBot="1"/>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
-      <c r="A3" s="124" t="s">
+    <row r="2" spans="1:4" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
-    </row>
-    <row r="4" spans="1:4" ht="33.75">
+      <c r="B3" s="148"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
+    </row>
+    <row r="4" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>58</v>
       </c>
@@ -3500,7 +4088,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="67.5">
+    <row r="5" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -3508,7 +4096,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -3516,7 +4104,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="22.5">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -3524,13 +4112,13 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="22.5">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>63</v>
       </c>
@@ -3540,7 +4128,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="33.75">
+    <row r="10" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -3552,7 +4140,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="56.25">
+    <row r="11" spans="1:4" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -3562,7 +4150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="79.5" thickBot="1">
+    <row r="12" spans="1:4" ht="79.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
@@ -3572,21 +4160,21 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="100.5" customHeight="1" thickBot="1">
+    <row r="13" spans="1:4" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:4" ht="15">
-      <c r="A14" s="124" t="s">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="126"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" s="148"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="149"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
@@ -3596,7 +4184,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="22.5">
+    <row r="16" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>75</v>
       </c>
@@ -3606,7 +4194,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="22.5">
+    <row r="17" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
@@ -3616,7 +4204,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>79</v>
       </c>
@@ -3626,7 +4214,7 @@
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="22.5">
+    <row r="19" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
@@ -3636,7 +4224,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="22.5">
+    <row r="20" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>83</v>
       </c>
@@ -3646,7 +4234,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>85</v>
       </c>
@@ -3656,7 +4244,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" ht="22.5">
+    <row r="22" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>87</v>
       </c>
@@ -3666,7 +4254,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="33.75">
+    <row r="23" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
@@ -3674,7 +4262,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" ht="33.75">
+    <row r="24" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
@@ -3682,7 +4270,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="22.5">
+    <row r="25" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
@@ -3690,7 +4278,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -3698,7 +4286,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="22.5">
+    <row r="27" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
@@ -3706,13 +4294,13 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="22.5">
+    <row r="29" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>94</v>
       </c>
@@ -3722,7 +4310,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="22.5">
+    <row r="30" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>96</v>
       </c>
@@ -3732,7 +4320,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="22.5">
+    <row r="31" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>98</v>
       </c>
@@ -3742,7 +4330,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" ht="33.75">
+    <row r="32" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>100</v>
       </c>
@@ -3752,7 +4340,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="33.75">
+    <row r="33" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>102</v>
       </c>
@@ -3762,7 +4350,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>104</v>
       </c>
@@ -3772,7 +4360,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="22.5">
+    <row r="35" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
@@ -3782,7 +4370,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="33.75">
+    <row r="36" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
@@ -3792,7 +4380,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="33.75">
+    <row r="37" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
@@ -3802,7 +4390,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45">
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
@@ -3812,7 +4400,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
@@ -3822,7 +4410,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="90">
+    <row r="40" spans="1:4" ht="90" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
@@ -3832,7 +4420,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45.75" thickBot="1">
+    <row r="41" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
@@ -3842,21 +4430,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="147.75" customHeight="1" thickBot="1">
+    <row r="42" spans="1:4" ht="147.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1">
-      <c r="A43" s="121" t="s">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="122"/>
-      <c r="C43" s="122"/>
-      <c r="D43" s="123"/>
-    </row>
-    <row r="44" spans="1:4" ht="45">
+      <c r="B43" s="145"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="146"/>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>121</v>
       </c>
@@ -3866,7 +4454,7 @@
       <c r="C44" s="95"/>
       <c r="D44" s="54"/>
     </row>
-    <row r="45" spans="1:4" ht="67.5">
+    <row r="45" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>123</v>
       </c>
@@ -3876,7 +4464,7 @@
       <c r="C45" s="95"/>
       <c r="D45" s="54"/>
     </row>
-    <row r="46" spans="1:4" ht="45">
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>125</v>
       </c>
@@ -3886,7 +4474,7 @@
       <c r="C46" s="95"/>
       <c r="D46" s="54"/>
     </row>
-    <row r="47" spans="1:4" ht="22.5">
+    <row r="47" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>127</v>
       </c>
@@ -3896,7 +4484,7 @@
       <c r="C47" s="95"/>
       <c r="D47" s="54"/>
     </row>
-    <row r="48" spans="1:4" ht="33.75">
+    <row r="48" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>129</v>
       </c>
@@ -3906,7 +4494,7 @@
       <c r="C48" s="95"/>
       <c r="D48" s="54"/>
     </row>
-    <row r="49" spans="1:4" ht="67.5">
+    <row r="49" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="95"/>
       <c r="C49" s="95" t="s">
@@ -3916,7 +4504,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="45">
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="95"/>
       <c r="C50" s="95" t="s">
@@ -3926,7 +4514,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="56.25">
+    <row r="51" spans="1:4" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="95"/>
       <c r="C51" s="95" t="s">
@@ -3936,7 +4524,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="102" thickBot="1">
+    <row r="52" spans="1:4" ht="102" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="96"/>
       <c r="C52" s="96" t="s">
@@ -3946,21 +4534,21 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="342" customHeight="1">
-      <c r="A53" s="127" t="s">
+    <row r="53" spans="1:4" ht="342" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="150" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="127"/>
-      <c r="C53" s="127"/>
-      <c r="D53" s="127"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1">
-      <c r="A54" s="128"/>
-      <c r="B54" s="128"/>
-      <c r="C54" s="128"/>
-      <c r="D54" s="128"/>
-    </row>
-    <row r="55" spans="1:4" ht="22.5">
+      <c r="B53" s="150"/>
+      <c r="C53" s="150"/>
+      <c r="D53" s="150"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="151"/>
+      <c r="D54" s="151"/>
+    </row>
+    <row r="55" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>140</v>
       </c>
@@ -3970,7 +4558,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="22.5">
+    <row r="56" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>142</v>
       </c>
@@ -3980,7 +4568,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="22.5">
+    <row r="57" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
         <v>144</v>
       </c>
@@ -3990,7 +4578,7 @@
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="22.5">
+    <row r="58" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>146</v>
       </c>
@@ -4000,7 +4588,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="33.75">
+    <row r="59" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>148</v>
       </c>
@@ -4010,7 +4598,7 @@
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="22.5">
+    <row r="60" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
@@ -4020,7 +4608,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="67.5">
+    <row r="61" spans="1:4" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
@@ -4030,7 +4618,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="22.5">
+    <row r="62" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
@@ -4054,144 +4642,324 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="129" t="s">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="161" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="163" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="B2" t="s">
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="164"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="152" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="171" t="s">
         <v>224</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="174" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2" s="174"/>
+      <c r="H2" s="175"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="153"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="116"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="153"/>
+      <c r="B4" s="117" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="116"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="153"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="108" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" s="115"/>
+      <c r="G5" s="98" t="s">
         <v>227</v>
       </c>
-      <c r="H2">
+      <c r="H5" s="100">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" t="s">
-        <v>226</v>
-      </c>
-      <c r="G3" t="s">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="153"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="111" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="102">
+        <v>4</v>
+      </c>
+      <c r="E6" s="105">
+        <v>8</v>
+      </c>
+      <c r="F6" s="115"/>
+      <c r="G6" s="101" t="s">
         <v>228</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H6" s="114" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="C6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="153"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="112" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="103">
+        <v>3</v>
+      </c>
+      <c r="E7" s="106">
+        <v>3</v>
+      </c>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="116"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="154"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="113" t="s">
         <v>233</v>
       </c>
-      <c r="D6" t="s">
-        <v>235</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D8" s="104"/>
+      <c r="E8" s="107" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="C7" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" t="s">
-        <v>234</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="119"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="155" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="99"/>
+      <c r="C10" s="158" t="s">
+        <v>248</v>
+      </c>
+      <c r="D10" s="159"/>
+      <c r="E10" s="159" t="s">
+        <v>240</v>
+      </c>
+      <c r="F10" s="159"/>
+      <c r="G10" s="159" t="s">
+        <v>241</v>
+      </c>
+      <c r="H10" s="160"/>
+    </row>
+    <row r="11" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="156"/>
+      <c r="B11" s="166" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="176" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="177"/>
+      <c r="E11" s="177" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" s="178"/>
+      <c r="G11" s="177" t="s">
+        <v>245</v>
+      </c>
+      <c r="H11" s="179"/>
+    </row>
+    <row r="12" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="156"/>
+      <c r="B12" s="167" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="180" t="s">
+        <v>266</v>
+      </c>
+      <c r="D12" s="181"/>
+      <c r="E12" s="181" t="s">
+        <v>246</v>
+      </c>
+      <c r="F12" s="182"/>
+      <c r="G12" s="181" t="s">
+        <v>247</v>
+      </c>
+      <c r="H12" s="183"/>
+    </row>
+    <row r="13" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="156"/>
+      <c r="B13" s="168" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="184" t="s">
+        <v>267</v>
+      </c>
+      <c r="D13" s="185"/>
+      <c r="E13" s="185" t="s">
+        <v>249</v>
+      </c>
+      <c r="F13" s="185"/>
+      <c r="G13" s="185" t="s">
+        <v>250</v>
+      </c>
+      <c r="H13" s="186"/>
+    </row>
+    <row r="14" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="156"/>
+      <c r="B14" s="168" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" s="184" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="185"/>
+      <c r="E14" s="185" t="s">
+        <v>251</v>
+      </c>
+      <c r="F14" s="185"/>
+      <c r="G14" s="185" t="s">
+        <v>252</v>
+      </c>
+      <c r="H14" s="187"/>
+    </row>
+    <row r="15" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="156"/>
+      <c r="B15" s="170" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" s="188" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>240</v>
-      </c>
-      <c r="C12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" t="s">
-        <v>241</v>
-      </c>
-      <c r="C14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="190"/>
+    </row>
+    <row r="16" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="156"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="191"/>
+      <c r="D16" s="191"/>
+      <c r="E16" s="191"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="191"/>
+      <c r="H16" s="191"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="156"/>
+      <c r="B17" s="165" t="s">
         <v>243</v>
       </c>
-      <c r="C15" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" t="s">
+      <c r="C17" s="192" t="s">
+        <v>253</v>
+      </c>
+      <c r="D17" s="193"/>
+      <c r="E17" s="194" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" s="195"/>
+      <c r="G17" s="195"/>
+      <c r="H17" s="196"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="157"/>
+      <c r="B18" s="169" t="s">
         <v>244</v>
       </c>
-      <c r="C16" t="s">
-        <v>245</v>
-      </c>
+      <c r="C18" s="197" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" s="198"/>
+      <c r="E18" s="199" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" s="199"/>
+      <c r="G18" s="199"/>
+      <c r="H18" s="200"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="28">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJ de certaines compétences
</commit_message>
<xml_diff>
--- a/Progression/Progression_Informatique_2014_2015.xlsx
+++ b/Progression/Progression_Informatique_2014_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="11670" windowHeight="7860" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="11670" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Progression_2014_2015" sheetId="1" r:id="rId1"/>
@@ -905,30 +905,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ANALYSER ET MODELISER </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Alg - C1, Alg - C3, Alg - C4, Alg - C5</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">MODELISER, CONCEVOIR, TRADUIRE
 </t>
     </r>
@@ -1457,6 +1433,30 @@
       </rPr>
       <t xml:space="preserve"> une situation
 Alg - C1, Alg - C3, Alg - C4, Alg - C5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ANALYSER ET MODELISER </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Alg - C1, Alg - C2  Alg - C4, Alg - C10,  Alg - C11,  Alg - C13 Alg - C14</t>
     </r>
   </si>
 </sst>
@@ -2632,6 +2632,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -2641,69 +2704,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2728,21 +2728,114 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2757,99 +2850,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3154,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3194,7 +3194,7 @@
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="149" t="s">
         <v>157</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -3213,7 +3213,7 @@
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="129"/>
+      <c r="B3" s="150"/>
       <c r="C3" s="25" t="s">
         <v>47</v>
       </c>
@@ -3228,7 +3228,7 @@
       <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="129"/>
+      <c r="B4" s="150"/>
       <c r="C4" s="31" t="s">
         <v>184</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="129"/>
+      <c r="B5" s="150"/>
       <c r="C5" s="25" t="s">
         <v>50</v>
       </c>
@@ -3262,7 +3262,7 @@
       <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="129"/>
+      <c r="B6" s="150"/>
       <c r="C6" s="25" t="s">
         <v>51</v>
       </c>
@@ -3284,7 +3284,7 @@
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="129"/>
+      <c r="B7" s="150"/>
       <c r="C7" s="25" t="s">
         <v>52</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="A8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="130"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="44" t="s">
         <v>52</v>
       </c>
@@ -3328,25 +3328,25 @@
       <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="131" t="s">
+      <c r="B10" s="128" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="133"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="130"/>
     </row>
     <row r="11" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="136"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="133"/>
     </row>
     <row r="12" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="49"/>
@@ -3359,7 +3359,7 @@
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="134" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -3382,7 +3382,7 @@
       <c r="A14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="138"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="36" t="s">
         <v>159</v>
       </c>
@@ -3393,22 +3393,22 @@
       <c r="F14" s="56"/>
       <c r="G14" s="29"/>
     </row>
-    <row r="15" spans="1:8" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="138"/>
+      <c r="B15" s="135"/>
       <c r="C15" s="36" t="s">
         <v>160</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>216</v>
+        <v>268</v>
       </c>
       <c r="E15" s="36" t="s">
         <v>199</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>204</v>
@@ -3418,12 +3418,12 @@
       <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="138"/>
-      <c r="C16" s="40" t="s">
+      <c r="B16" s="135"/>
+      <c r="C16" s="36" t="s">
         <v>161</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E16" s="55"/>
       <c r="F16" s="56"/>
@@ -3433,18 +3433,18 @@
       <c r="A17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="135"/>
+      <c r="C17" s="36" t="s">
         <v>161</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="36" t="s">
         <v>199</v>
       </c>
       <c r="F17" s="54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>205</v>
@@ -3454,31 +3454,31 @@
       <c r="A18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="138"/>
+      <c r="B18" s="135"/>
       <c r="C18" s="40" t="s">
         <v>162</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E18" s="36" t="s">
         <v>199</v>
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="139"/>
+      <c r="B19" s="136"/>
       <c r="C19" s="58" t="s">
         <v>162</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E19" s="60" t="s">
         <v>194</v>
@@ -3497,25 +3497,25 @@
       <c r="A21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="128" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="133"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="130"/>
     </row>
     <row r="22" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="134"/>
-      <c r="C22" s="135"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="136"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="133"/>
     </row>
     <row r="23" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="49"/>
@@ -3528,7 +3528,7 @@
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="137" t="s">
+      <c r="B24" s="134" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -3547,7 +3547,7 @@
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="138"/>
+      <c r="B25" s="135"/>
       <c r="C25" s="36" t="s">
         <v>168</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="A26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="139"/>
+      <c r="B26" s="136"/>
       <c r="C26" s="64" t="s">
         <v>177</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="A27" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="140" t="s">
+      <c r="B27" s="137" t="s">
         <v>158</v>
       </c>
       <c r="C27" s="65" t="s">
@@ -3598,7 +3598,7 @@
       <c r="A28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="140"/>
+      <c r="B28" s="137"/>
       <c r="C28" s="68" t="s">
         <v>170</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="A29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="140"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="68" t="s">
         <v>171</v>
       </c>
@@ -3634,7 +3634,7 @@
       <c r="A30" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="141"/>
+      <c r="B30" s="138"/>
       <c r="C30" s="71" t="s">
         <v>171</v>
       </c>
@@ -3658,25 +3658,25 @@
       <c r="A32" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
-      <c r="G32" s="133"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="129"/>
+      <c r="F32" s="129"/>
+      <c r="G32" s="130"/>
     </row>
     <row r="33" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="134"/>
-      <c r="C33" s="135"/>
-      <c r="D33" s="135"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="135"/>
-      <c r="G33" s="136"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="133"/>
     </row>
     <row r="34" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="49"/>
@@ -3689,20 +3689,20 @@
       <c r="A35" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="149" t="s">
+      <c r="B35" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="150"/>
-      <c r="D35" s="150"/>
-      <c r="E35" s="150"/>
-      <c r="F35" s="150"/>
-      <c r="G35" s="151"/>
+      <c r="C35" s="147"/>
+      <c r="D35" s="147"/>
+      <c r="E35" s="147"/>
+      <c r="F35" s="147"/>
+      <c r="G35" s="148"/>
     </row>
     <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="146" t="s">
+      <c r="B36" s="143" t="s">
         <v>158</v>
       </c>
       <c r="C36" s="74" t="s">
@@ -3721,7 +3721,7 @@
       <c r="A37" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="147"/>
+      <c r="B37" s="144"/>
       <c r="C37" s="76" t="s">
         <v>172</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="A38" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="147"/>
+      <c r="B38" s="144"/>
       <c r="C38" s="78" t="s">
         <v>174</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="A39" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="147"/>
+      <c r="B39" s="144"/>
       <c r="C39" s="78" t="s">
         <v>173</v>
       </c>
@@ -3772,7 +3772,7 @@
       <c r="A40" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="147"/>
+      <c r="B40" s="144"/>
       <c r="C40" s="78" t="s">
         <v>173</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="A41" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="148"/>
+      <c r="B41" s="145"/>
       <c r="C41" s="79" t="s">
         <v>175</v>
       </c>
@@ -3815,25 +3815,25 @@
       <c r="A43" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="131" t="s">
+      <c r="B43" s="128" t="s">
         <v>166</v>
       </c>
-      <c r="C43" s="132"/>
-      <c r="D43" s="132"/>
-      <c r="E43" s="132"/>
-      <c r="F43" s="132"/>
-      <c r="G43" s="133"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="130"/>
     </row>
     <row r="44" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="134"/>
-      <c r="C44" s="135"/>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="136"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="132"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="132"/>
+      <c r="F44" s="132"/>
+      <c r="G44" s="133"/>
     </row>
     <row r="45" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="49"/>
@@ -3846,7 +3846,7 @@
       <c r="A46" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="145" t="s">
+      <c r="B46" s="142" t="s">
         <v>158</v>
       </c>
       <c r="C46" s="83" t="s">
@@ -3863,7 +3863,7 @@
       <c r="A47" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="140"/>
+      <c r="B47" s="137"/>
       <c r="C47" s="69" t="s">
         <v>179</v>
       </c>
@@ -3878,7 +3878,7 @@
       <c r="A48" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="141"/>
+      <c r="B48" s="138"/>
       <c r="C48" s="69" t="s">
         <v>179</v>
       </c>
@@ -3893,14 +3893,14 @@
       <c r="A49" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="142" t="s">
+      <c r="B49" s="139" t="s">
         <v>167</v>
       </c>
       <c r="C49" s="85" t="s">
         <v>178</v>
       </c>
       <c r="D49" s="54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E49" s="55" t="s">
         <v>180</v>
@@ -3912,12 +3912,12 @@
       <c r="A50" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="143"/>
+      <c r="B50" s="140"/>
       <c r="C50" s="85" t="s">
         <v>176</v>
       </c>
       <c r="D50" s="54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E50" s="55" t="s">
         <v>181</v>
@@ -3931,12 +3931,12 @@
       <c r="A51" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="143"/>
+      <c r="B51" s="140"/>
       <c r="C51" s="85" t="s">
         <v>176</v>
       </c>
       <c r="D51" s="54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E51" s="55" t="s">
         <v>180</v>
@@ -3948,7 +3948,7 @@
       <c r="A52" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="144"/>
+      <c r="B52" s="141"/>
       <c r="C52" s="86" t="s">
         <v>179</v>
       </c>
@@ -3990,6 +3990,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B21:G22"/>
+    <mergeCell ref="B32:G33"/>
     <mergeCell ref="B43:G44"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="B27:B30"/>
@@ -3997,11 +4002,6 @@
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B36:B41"/>
     <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="B21:G22"/>
-    <mergeCell ref="B32:G33"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4058,8 +4058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D62"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4645,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4657,39 +4657,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="197" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="198"/>
+      <c r="C1" s="194" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="162" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="163"/>
+      <c r="D1" s="194"/>
+      <c r="E1" s="194"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="194"/>
+      <c r="H1" s="195"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180" t="s">
-        <v>257</v>
-      </c>
-      <c r="B2" s="188" t="s">
+      <c r="A2" s="164" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="172" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="126" t="s">
+      <c r="F2" s="170" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="186" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="171"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="181"/>
+      <c r="A3" s="165"/>
       <c r="B3" s="115"/>
       <c r="C3" s="115"/>
       <c r="D3" s="115"/>
@@ -4699,9 +4699,9 @@
       <c r="H3" s="116"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="181"/>
+      <c r="A4" s="165"/>
       <c r="B4" s="117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C4" s="115"/>
       <c r="D4" s="115"/>
@@ -4711,30 +4711,30 @@
       <c r="H4" s="116"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="181"/>
+      <c r="A5" s="165"/>
       <c r="B5" s="115"/>
       <c r="C5" s="108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="109" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E5" s="110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F5" s="115"/>
       <c r="G5" s="98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H5" s="100">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="181"/>
+      <c r="A6" s="165"/>
       <c r="B6" s="115"/>
       <c r="C6" s="111" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" s="102">
         <v>4</v>
@@ -4744,17 +4744,17 @@
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="101" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="114" t="s">
         <v>228</v>
       </c>
-      <c r="H6" s="114" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="181"/>
+      <c r="A7" s="165"/>
       <c r="B7" s="115"/>
       <c r="C7" s="112" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D7" s="103">
         <v>3</v>
@@ -4767,14 +4767,14 @@
       <c r="H7" s="116"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="182"/>
+      <c r="A8" s="166"/>
       <c r="B8" s="118"/>
       <c r="C8" s="113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D8" s="104"/>
       <c r="E8" s="107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F8" s="118"/>
       <c r="G8" s="118"/>
@@ -4782,111 +4782,111 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="183" t="s">
-        <v>258</v>
+      <c r="A10" s="167" t="s">
+        <v>257</v>
       </c>
       <c r="B10" s="99"/>
-      <c r="C10" s="196" t="s">
+      <c r="C10" s="181" t="s">
+        <v>247</v>
+      </c>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="182"/>
+      <c r="G10" s="182" t="s">
+        <v>240</v>
+      </c>
+      <c r="H10" s="183"/>
+    </row>
+    <row r="11" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="168"/>
+      <c r="B11" s="121" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="199" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" s="185"/>
+      <c r="G11" s="184" t="s">
+        <v>244</v>
+      </c>
+      <c r="H11" s="196"/>
+    </row>
+    <row r="12" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="168"/>
+      <c r="B12" s="122" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="200" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="186"/>
+      <c r="E12" s="186" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="187"/>
+      <c r="G12" s="186" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" s="192"/>
+    </row>
+    <row r="13" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="168"/>
+      <c r="B13" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="193" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="188"/>
+      <c r="E13" s="188" t="s">
         <v>248</v>
       </c>
-      <c r="D10" s="197"/>
-      <c r="E10" s="197" t="s">
-        <v>240</v>
-      </c>
-      <c r="F10" s="197"/>
-      <c r="G10" s="197" t="s">
-        <v>241</v>
-      </c>
-      <c r="H10" s="198"/>
-    </row>
-    <row r="11" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
-      <c r="B11" s="121" t="s">
-        <v>260</v>
-      </c>
-      <c r="C11" s="168" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="164"/>
-      <c r="E11" s="164" t="s">
-        <v>242</v>
-      </c>
-      <c r="F11" s="199"/>
-      <c r="G11" s="164" t="s">
-        <v>245</v>
-      </c>
-      <c r="H11" s="165"/>
-    </row>
-    <row r="12" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="184"/>
-      <c r="B12" s="122" t="s">
+      <c r="F13" s="188"/>
+      <c r="G13" s="188" t="s">
+        <v>249</v>
+      </c>
+      <c r="H13" s="191"/>
+    </row>
+    <row r="14" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="168"/>
+      <c r="B14" s="123" t="s">
         <v>261</v>
       </c>
-      <c r="C12" s="169" t="s">
-        <v>266</v>
-      </c>
-      <c r="D12" s="170"/>
-      <c r="E12" s="170" t="s">
-        <v>246</v>
-      </c>
-      <c r="F12" s="200"/>
-      <c r="G12" s="170" t="s">
-        <v>247</v>
-      </c>
-      <c r="H12" s="175"/>
-    </row>
-    <row r="13" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="184"/>
-      <c r="B13" s="123" t="s">
+      <c r="C14" s="193" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="188"/>
+      <c r="E14" s="188" t="s">
+        <v>250</v>
+      </c>
+      <c r="F14" s="188"/>
+      <c r="G14" s="188" t="s">
+        <v>251</v>
+      </c>
+      <c r="H14" s="190"/>
+    </row>
+    <row r="15" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="168"/>
+      <c r="B15" s="125" t="s">
         <v>263</v>
       </c>
-      <c r="C13" s="160" t="s">
-        <v>267</v>
-      </c>
-      <c r="D13" s="161"/>
-      <c r="E13" s="161" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="161"/>
-      <c r="G13" s="161" t="s">
-        <v>250</v>
-      </c>
-      <c r="H13" s="174"/>
-    </row>
-    <row r="14" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="184"/>
-      <c r="B14" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="C14" s="160" t="s">
-        <v>268</v>
-      </c>
-      <c r="D14" s="161"/>
-      <c r="E14" s="161" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" s="161"/>
-      <c r="G14" s="161" t="s">
-        <v>252</v>
-      </c>
-      <c r="H14" s="173"/>
-    </row>
-    <row r="15" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="184"/>
-      <c r="B15" s="125" t="s">
-        <v>264</v>
-      </c>
-      <c r="C15" s="195" t="s">
-        <v>239</v>
-      </c>
-      <c r="D15" s="171"/>
-      <c r="E15" s="171"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="172"/>
+      <c r="C15" s="179" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="180"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="189"/>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="184"/>
+      <c r="A16" s="168"/>
       <c r="B16" s="97"/>
       <c r="C16" s="127"/>
       <c r="D16" s="127"/>
@@ -4896,39 +4896,51 @@
       <c r="H16" s="127"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="184"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="120" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="160" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="161"/>
+      <c r="E17" s="176" t="s">
+        <v>253</v>
+      </c>
+      <c r="F17" s="177"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="169"/>
+      <c r="B18" s="124" t="s">
         <v>243</v>
       </c>
-      <c r="C17" s="176" t="s">
-        <v>253</v>
-      </c>
-      <c r="D17" s="177"/>
-      <c r="E17" s="192" t="s">
+      <c r="C18" s="162" t="s">
         <v>254</v>
       </c>
-      <c r="F17" s="193"/>
-      <c r="G17" s="193"/>
-      <c r="H17" s="194"/>
-    </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="185"/>
-      <c r="B18" s="124" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="178" t="s">
-        <v>255</v>
-      </c>
-      <c r="D18" s="179"/>
-      <c r="E18" s="190" t="s">
-        <v>259</v>
-      </c>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
-      <c r="H18" s="191"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="174" t="s">
+        <v>258</v>
+      </c>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
+      <c r="H18" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A2:A8"/>
@@ -4945,18 +4957,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Ajout des compétences de seconde année
</commit_message>
<xml_diff>
--- a/Progression/Progression_Informatique_2014_2015.xlsx
+++ b/Progression/Progression_Informatique_2014_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="11670" windowHeight="7860"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="11670" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Progression_2014_2015" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="284">
   <si>
     <t>01/09/2014
 au
@@ -1483,6 +1483,33 @@
   <si>
     <t>TP EO
 BDD Aéroports du monde</t>
+  </si>
+  <si>
+    <t>Partie 5 - Algorithme et programmation - Suite</t>
+  </si>
+  <si>
+    <t>Alg - C15</t>
+  </si>
+  <si>
+    <t>Récursivité - Avantages et inconvénients</t>
+  </si>
+  <si>
+    <t>Alg - C16</t>
+  </si>
+  <si>
+    <t>Piles - Algorithmes de manipulation : fonctions «push» et «pop».</t>
+  </si>
+  <si>
+    <t>Alg - C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tris d’un tableau à une dimension de
+valeurs numériques. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri par insertion, tri rapide (ou « quicksort »), tri par fusion.
+Application à la recherche de la médiane d’une liste de nombres. 
+On étudie et on compare ces algorithmes de tri du point de vue des complexités temporelles dans le meilleur et dans le pire cas. </t>
   </si>
 </sst>
 </file>
@@ -2328,7 +2355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2657,6 +2684,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2720,15 +2759,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2747,11 +2777,53 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2813,9 +2885,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2826,58 +2895,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3185,7 +3222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -3225,7 +3262,7 @@
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="129" t="s">
         <v>157</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -3244,7 +3281,7 @@
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="150"/>
+      <c r="B3" s="130"/>
       <c r="C3" s="25" t="s">
         <v>47</v>
       </c>
@@ -3259,7 +3296,7 @@
       <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="150"/>
+      <c r="B4" s="130"/>
       <c r="C4" s="31" t="s">
         <v>182</v>
       </c>
@@ -3276,7 +3313,7 @@
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="150"/>
+      <c r="B5" s="130"/>
       <c r="C5" s="25" t="s">
         <v>50</v>
       </c>
@@ -3293,7 +3330,7 @@
       <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="150"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="25" t="s">
         <v>51</v>
       </c>
@@ -3315,7 +3352,7 @@
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="150"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="25" t="s">
         <v>52</v>
       </c>
@@ -3337,7 +3374,7 @@
       <c r="A8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="151"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="44" t="s">
         <v>52</v>
       </c>
@@ -3359,25 +3396,25 @@
       <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="128" t="s">
+      <c r="B10" s="132" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="130"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="134"/>
     </row>
     <row r="11" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="131"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="133"/>
+      <c r="B11" s="135"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="137"/>
     </row>
     <row r="12" spans="1:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="49"/>
@@ -3390,7 +3427,7 @@
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="138" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -3413,7 +3450,7 @@
       <c r="A14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="135"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="36" t="s">
         <v>159</v>
       </c>
@@ -3428,7 +3465,7 @@
       <c r="A15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="135"/>
+      <c r="B15" s="139"/>
       <c r="C15" s="36" t="s">
         <v>160</v>
       </c>
@@ -3449,7 +3486,7 @@
       <c r="A16" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="135"/>
+      <c r="B16" s="139"/>
       <c r="C16" s="36" t="s">
         <v>161</v>
       </c>
@@ -3464,7 +3501,7 @@
       <c r="A17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="135"/>
+      <c r="B17" s="139"/>
       <c r="C17" s="36" t="s">
         <v>161</v>
       </c>
@@ -3485,7 +3522,7 @@
       <c r="A18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="135"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="40" t="s">
         <v>162</v>
       </c>
@@ -3504,7 +3541,7 @@
       <c r="A19" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="136"/>
+      <c r="B19" s="140"/>
       <c r="C19" s="58" t="s">
         <v>162</v>
       </c>
@@ -3528,25 +3565,25 @@
       <c r="A21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="132" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="129"/>
-      <c r="G21" s="130"/>
+      <c r="C21" s="133"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="134"/>
     </row>
     <row r="22" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="131"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="133"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="137"/>
     </row>
     <row r="23" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="49"/>
@@ -3559,7 +3596,7 @@
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="134" t="s">
+      <c r="B24" s="138" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -3578,7 +3615,7 @@
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="135"/>
+      <c r="B25" s="139"/>
       <c r="C25" s="36" t="s">
         <v>168</v>
       </c>
@@ -3593,7 +3630,7 @@
       <c r="A26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="136"/>
+      <c r="B26" s="140"/>
       <c r="C26" s="63" t="s">
         <v>177</v>
       </c>
@@ -3610,7 +3647,7 @@
       <c r="A27" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="137" t="s">
+      <c r="B27" s="141" t="s">
         <v>158</v>
       </c>
       <c r="C27" s="64" t="s">
@@ -3629,7 +3666,7 @@
       <c r="A28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="137"/>
+      <c r="B28" s="141"/>
       <c r="C28" s="67" t="s">
         <v>170</v>
       </c>
@@ -3646,7 +3683,7 @@
       <c r="A29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="137"/>
+      <c r="B29" s="141"/>
       <c r="C29" s="67" t="s">
         <v>171</v>
       </c>
@@ -3665,7 +3702,7 @@
       <c r="A30" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="138"/>
+      <c r="B30" s="142"/>
       <c r="C30" s="70" t="s">
         <v>171</v>
       </c>
@@ -3691,25 +3728,25 @@
       <c r="A32" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="128" t="s">
+      <c r="B32" s="132" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="129"/>
-      <c r="D32" s="129"/>
-      <c r="E32" s="129"/>
-      <c r="F32" s="129"/>
-      <c r="G32" s="130"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="134"/>
     </row>
     <row r="33" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="131"/>
-      <c r="C33" s="132"/>
-      <c r="D33" s="132"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="133"/>
+      <c r="B33" s="135"/>
+      <c r="C33" s="136"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="137"/>
     </row>
     <row r="34" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C34" s="49"/>
@@ -3722,20 +3759,20 @@
       <c r="A35" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="146" t="s">
+      <c r="B35" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="147"/>
-      <c r="F35" s="147"/>
-      <c r="G35" s="148"/>
+      <c r="C35" s="151"/>
+      <c r="D35" s="151"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151"/>
+      <c r="G35" s="152"/>
     </row>
     <row r="36" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="143" t="s">
+      <c r="B36" s="147" t="s">
         <v>158</v>
       </c>
       <c r="C36" s="73" t="s">
@@ -3754,7 +3791,7 @@
       <c r="A37" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="144"/>
+      <c r="B37" s="148"/>
       <c r="C37" s="75" t="s">
         <v>172</v>
       </c>
@@ -3771,7 +3808,7 @@
       <c r="A38" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="144"/>
+      <c r="B38" s="148"/>
       <c r="C38" s="77" t="s">
         <v>174</v>
       </c>
@@ -3788,7 +3825,7 @@
       <c r="A39" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="144"/>
+      <c r="B39" s="148"/>
       <c r="C39" s="77" t="s">
         <v>173</v>
       </c>
@@ -3805,7 +3842,7 @@
       <c r="A40" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="144"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="77" t="s">
         <v>173</v>
       </c>
@@ -3824,7 +3861,7 @@
       <c r="A41" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="145"/>
+      <c r="B41" s="149"/>
       <c r="C41" s="78" t="s">
         <v>175</v>
       </c>
@@ -3848,25 +3885,25 @@
       <c r="A43" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="128" t="s">
+      <c r="B43" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="C43" s="129"/>
-      <c r="D43" s="129"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="130"/>
+      <c r="C43" s="133"/>
+      <c r="D43" s="133"/>
+      <c r="E43" s="133"/>
+      <c r="F43" s="133"/>
+      <c r="G43" s="134"/>
     </row>
     <row r="44" spans="1:7" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="131"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="132"/>
-      <c r="E44" s="132"/>
-      <c r="F44" s="132"/>
-      <c r="G44" s="133"/>
+      <c r="B44" s="135"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="137"/>
     </row>
     <row r="45" spans="1:7" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="49"/>
@@ -3879,7 +3916,7 @@
       <c r="A46" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="142" t="s">
+      <c r="B46" s="146" t="s">
         <v>158</v>
       </c>
       <c r="C46" s="82" t="s">
@@ -3896,12 +3933,12 @@
       <c r="A47" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="137"/>
+      <c r="B47" s="141"/>
       <c r="C47" s="68" t="s">
         <v>271</v>
       </c>
       <c r="D47" s="54"/>
-      <c r="E47" s="201" t="s">
+      <c r="E47" s="128" t="s">
         <v>272</v>
       </c>
       <c r="F47" s="56"/>
@@ -3911,12 +3948,12 @@
       <c r="A48" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="138"/>
+      <c r="B48" s="142"/>
       <c r="C48" s="68" t="s">
         <v>270</v>
       </c>
       <c r="D48" s="54"/>
-      <c r="E48" s="201" t="s">
+      <c r="E48" s="128" t="s">
         <v>273</v>
       </c>
       <c r="F48" s="56"/>
@@ -3926,7 +3963,7 @@
       <c r="A49" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="143" t="s">
         <v>167</v>
       </c>
       <c r="C49" s="84" t="s">
@@ -3935,7 +3972,7 @@
       <c r="D49" s="54" t="s">
         <v>217</v>
       </c>
-      <c r="E49" s="201" t="s">
+      <c r="E49" s="128" t="s">
         <v>274</v>
       </c>
       <c r="F49" s="56"/>
@@ -3945,14 +3982,14 @@
       <c r="A50" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="140"/>
+      <c r="B50" s="144"/>
       <c r="C50" s="84" t="s">
         <v>176</v>
       </c>
       <c r="D50" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="201" t="s">
+      <c r="E50" s="128" t="s">
         <v>275</v>
       </c>
       <c r="F50" s="56"/>
@@ -3964,7 +4001,7 @@
       <c r="A51" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="140"/>
+      <c r="B51" s="144"/>
       <c r="C51" s="84" t="s">
         <v>176</v>
       </c>
@@ -3977,7 +4014,7 @@
       <c r="A52" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="141"/>
+      <c r="B52" s="145"/>
       <c r="C52" s="85"/>
       <c r="D52" s="89"/>
       <c r="E52" s="46"/>
@@ -4013,11 +4050,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="B21:G22"/>
-    <mergeCell ref="B32:G33"/>
     <mergeCell ref="B43:G44"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="B27:B30"/>
@@ -4025,6 +4057,11 @@
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B36:B41"/>
     <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B21:G22"/>
+    <mergeCell ref="B32:G33"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4036,7 +4073,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4079,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D62"/>
+  <dimension ref="A2:D67"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="90" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4094,12 +4131,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="156" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="157"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="158"/>
     </row>
     <row r="4" spans="1:4" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -4183,19 +4220,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="155" t="s">
+      <c r="A14" s="156" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="156"/>
-      <c r="C14" s="156"/>
-      <c r="D14" s="157"/>
+      <c r="B14" s="157"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="158"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -4453,19 +4490,19 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="147.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="152" t="s">
+      <c r="A43" s="153" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="153"/>
-      <c r="C43" s="153"/>
-      <c r="D43" s="154"/>
+      <c r="B43" s="154"/>
+      <c r="C43" s="154"/>
+      <c r="D43" s="155"/>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
@@ -4557,29 +4594,28 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="342" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="158" t="s">
+    <row r="53" spans="1:4" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="200"/>
+      <c r="C53" s="200"/>
+      <c r="D53" s="200"/>
+    </row>
+    <row r="54" spans="1:4" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="203" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="158"/>
-      <c r="C53" s="158"/>
-      <c r="D53" s="158"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="159"/>
-      <c r="B54" s="159"/>
-      <c r="C54" s="159"/>
-      <c r="D54" s="159"/>
+      <c r="B54" s="204"/>
+      <c r="C54" s="204"/>
+      <c r="D54" s="205"/>
     </row>
     <row r="55" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="201" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="202" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="202"/>
+      <c r="D55" s="202"/>
     </row>
     <row r="56" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
@@ -4641,7 +4677,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5" t="s">
@@ -4651,12 +4687,58 @@
         <v>155</v>
       </c>
     </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="200"/>
+      <c r="C63" s="200"/>
+      <c r="D63" s="200"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="203" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" s="204"/>
+      <c r="C64" s="204"/>
+      <c r="D64" s="205"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="201" t="s">
+        <v>277</v>
+      </c>
+      <c r="B65" s="202" t="s">
+        <v>278</v>
+      </c>
+      <c r="C65" s="202"/>
+      <c r="D65" s="202"/>
+    </row>
+    <row r="66" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="1:4" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D67" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A64:D64"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A53:D54"/>
+    <mergeCell ref="A54:D54"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4680,39 +4762,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="165" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="194" t="s">
+      <c r="B1" s="166"/>
+      <c r="C1" s="161" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="194"/>
-      <c r="H1" s="195"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="162"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="179" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="187" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
       <c r="E2" s="125" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="170" t="s">
+      <c r="F2" s="185" t="s">
         <v>221</v>
       </c>
-      <c r="G2" s="170"/>
-      <c r="H2" s="171"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="186"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="165"/>
+      <c r="A3" s="180"/>
       <c r="B3" s="114"/>
       <c r="C3" s="114"/>
       <c r="D3" s="114"/>
@@ -4722,7 +4804,7 @@
       <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="165"/>
+      <c r="A4" s="180"/>
       <c r="B4" s="116" t="s">
         <v>251</v>
       </c>
@@ -4734,7 +4816,7 @@
       <c r="H4" s="115"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="165"/>
+      <c r="A5" s="180"/>
       <c r="B5" s="114"/>
       <c r="C5" s="107" t="s">
         <v>227</v>
@@ -4754,7 +4836,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="165"/>
+      <c r="A6" s="180"/>
       <c r="B6" s="114"/>
       <c r="C6" s="110" t="s">
         <v>230</v>
@@ -4774,7 +4856,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="165"/>
+      <c r="A7" s="180"/>
       <c r="B7" s="114"/>
       <c r="C7" s="111" t="s">
         <v>231</v>
@@ -4790,7 +4872,7 @@
       <c r="H7" s="115"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="166"/>
+      <c r="A8" s="181"/>
       <c r="B8" s="117"/>
       <c r="C8" s="112" t="s">
         <v>228</v>
@@ -4805,111 +4887,111 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="167" t="s">
+      <c r="A10" s="182" t="s">
         <v>253</v>
       </c>
       <c r="B10" s="98"/>
-      <c r="C10" s="181" t="s">
+      <c r="C10" s="195" t="s">
         <v>243</v>
       </c>
-      <c r="D10" s="182"/>
-      <c r="E10" s="182" t="s">
+      <c r="D10" s="196"/>
+      <c r="E10" s="196" t="s">
         <v>235</v>
       </c>
-      <c r="F10" s="182"/>
-      <c r="G10" s="182" t="s">
+      <c r="F10" s="196"/>
+      <c r="G10" s="196" t="s">
         <v>236</v>
       </c>
-      <c r="H10" s="183"/>
+      <c r="H10" s="197"/>
     </row>
     <row r="11" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="168"/>
+      <c r="A11" s="183"/>
       <c r="B11" s="120" t="s">
         <v>255</v>
       </c>
-      <c r="C11" s="199" t="s">
+      <c r="C11" s="167" t="s">
         <v>260</v>
       </c>
-      <c r="D11" s="184"/>
-      <c r="E11" s="184" t="s">
+      <c r="D11" s="163"/>
+      <c r="E11" s="163" t="s">
         <v>237</v>
       </c>
-      <c r="F11" s="185"/>
-      <c r="G11" s="184" t="s">
+      <c r="F11" s="198"/>
+      <c r="G11" s="163" t="s">
         <v>240</v>
       </c>
-      <c r="H11" s="196"/>
+      <c r="H11" s="164"/>
     </row>
     <row r="12" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="168"/>
+      <c r="A12" s="183"/>
       <c r="B12" s="121" t="s">
         <v>256</v>
       </c>
-      <c r="C12" s="200" t="s">
+      <c r="C12" s="168" t="s">
         <v>261</v>
       </c>
-      <c r="D12" s="186"/>
-      <c r="E12" s="186" t="s">
+      <c r="D12" s="169"/>
+      <c r="E12" s="169" t="s">
         <v>241</v>
       </c>
-      <c r="F12" s="187"/>
-      <c r="G12" s="186" t="s">
+      <c r="F12" s="199"/>
+      <c r="G12" s="169" t="s">
         <v>242</v>
       </c>
-      <c r="H12" s="192"/>
+      <c r="H12" s="174"/>
     </row>
     <row r="13" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="168"/>
+      <c r="A13" s="183"/>
       <c r="B13" s="122" t="s">
         <v>258</v>
       </c>
-      <c r="C13" s="193" t="s">
+      <c r="C13" s="159" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="188"/>
-      <c r="E13" s="188" t="s">
+      <c r="D13" s="160"/>
+      <c r="E13" s="160" t="s">
         <v>244</v>
       </c>
-      <c r="F13" s="188"/>
-      <c r="G13" s="188" t="s">
+      <c r="F13" s="160"/>
+      <c r="G13" s="160" t="s">
         <v>245</v>
       </c>
-      <c r="H13" s="191"/>
+      <c r="H13" s="173"/>
     </row>
     <row r="14" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="168"/>
+      <c r="A14" s="183"/>
       <c r="B14" s="122" t="s">
         <v>257</v>
       </c>
-      <c r="C14" s="193" t="s">
+      <c r="C14" s="159" t="s">
         <v>263</v>
       </c>
-      <c r="D14" s="188"/>
-      <c r="E14" s="188" t="s">
+      <c r="D14" s="160"/>
+      <c r="E14" s="160" t="s">
         <v>246</v>
       </c>
-      <c r="F14" s="188"/>
-      <c r="G14" s="188" t="s">
+      <c r="F14" s="160"/>
+      <c r="G14" s="160" t="s">
         <v>247</v>
       </c>
-      <c r="H14" s="190"/>
+      <c r="H14" s="172"/>
     </row>
     <row r="15" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="168"/>
+      <c r="A15" s="183"/>
       <c r="B15" s="124" t="s">
         <v>259</v>
       </c>
-      <c r="C15" s="179" t="s">
+      <c r="C15" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="D15" s="180"/>
-      <c r="E15" s="180"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="189"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="171"/>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="168"/>
+      <c r="A16" s="183"/>
       <c r="B16" s="96"/>
       <c r="C16" s="126"/>
       <c r="D16" s="126"/>
@@ -4919,51 +5001,39 @@
       <c r="H16" s="126"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="168"/>
+      <c r="A17" s="183"/>
       <c r="B17" s="119" t="s">
         <v>238</v>
       </c>
-      <c r="C17" s="160" t="s">
+      <c r="C17" s="175" t="s">
         <v>248</v>
       </c>
-      <c r="D17" s="161"/>
-      <c r="E17" s="176" t="s">
+      <c r="D17" s="176"/>
+      <c r="E17" s="191" t="s">
         <v>249</v>
       </c>
-      <c r="F17" s="177"/>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
+      <c r="F17" s="192"/>
+      <c r="G17" s="192"/>
+      <c r="H17" s="193"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="169"/>
+      <c r="A18" s="184"/>
       <c r="B18" s="123" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="162" t="s">
+      <c r="C18" s="177" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="163"/>
-      <c r="E18" s="174" t="s">
+      <c r="D18" s="178"/>
+      <c r="E18" s="189" t="s">
         <v>254</v>
       </c>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="175"/>
+      <c r="F18" s="189"/>
+      <c r="G18" s="189"/>
+      <c r="H18" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A2:A8"/>
@@ -4980,6 +5050,18 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>